<commit_message>
Added unit tests for utils and distractor analysis.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/ex1/tables/distractors_items.xlsx
+++ b/tests/testthat/fixtures/ex1/tables/distractors_items.xlsx
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">grk10001</t>
   </si>
@@ -40,25 +37,25 @@
     <t xml:space="preserve">rit</t>
   </si>
   <si>
+    <t xml:space="preserve">*1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grk10002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grk10003</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grk10002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grk10003</t>
   </si>
   <si>
     <t xml:space="preserve">*2</t>
@@ -445,64 +442,49 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>808</v>
       </c>
       <c r="C2" t="n">
-        <v>787</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.31</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>62</v>
       </c>
       <c r="C3" t="n">
-        <v>58</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.222</v>
+        <v>-0.232</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>49</v>
       </c>
       <c r="C4" t="n">
-        <v>49</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.116</v>
+        <v>-0.103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>45</v>
       </c>
       <c r="C5" t="n">
-        <v>43</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.165</v>
+        <v>-0.18</v>
       </c>
     </row>
   </sheetData>
@@ -521,72 +503,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>152</v>
       </c>
       <c r="C2" t="n">
-        <v>142</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.091</v>
+        <v>-0.097</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>203</v>
       </c>
       <c r="C3" t="n">
-        <v>197</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.2</v>
+        <v>-0.176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>175</v>
       </c>
       <c r="C4" t="n">
-        <v>170</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.19</v>
+        <v>-0.194</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="n">
+        <v>365</v>
       </c>
       <c r="C5" t="n">
-        <v>337</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.398</v>
+        <v>0.38</v>
       </c>
     </row>
   </sheetData>
@@ -605,72 +572,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>183</v>
       </c>
       <c r="C2" t="n">
-        <v>178</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.192</v>
+        <v>-0.194</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>189</v>
       </c>
       <c r="C3" t="n">
-        <v>171</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.141</v>
+        <v>-0.158</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>297</v>
       </c>
       <c r="C4" t="n">
-        <v>285</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.402</v>
+        <v>0.415</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>173</v>
       </c>
       <c r="C5" t="n">
-        <v>167</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.136</v>
+        <v>-0.13</v>
       </c>
     </row>
   </sheetData>
@@ -689,72 +641,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>227</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.363</v>
+        <v>0.351</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>185</v>
       </c>
       <c r="C3" t="n">
-        <v>174</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.177</v>
+        <v>-0.188</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>179</v>
       </c>
       <c r="C4" t="n">
-        <v>179</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.105</v>
+        <v>-0.079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>171</v>
       </c>
       <c r="C5" t="n">
-        <v>155</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.117</v>
+        <v>-0.122</v>
       </c>
     </row>
   </sheetData>
@@ -773,72 +710,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>180</v>
       </c>
       <c r="C2" t="n">
-        <v>178</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.07</v>
+        <v>-0.116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>173</v>
       </c>
       <c r="C3" t="n">
-        <v>160</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.105</v>
+        <v>-0.123</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>163</v>
       </c>
       <c r="C4" t="n">
-        <v>154</v>
-      </c>
-      <c r="D4" t="n">
         <v>0.343</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>163</v>
       </c>
       <c r="C5" t="n">
-        <v>152</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.165</v>
+        <v>-0.098</v>
       </c>
     </row>
   </sheetData>
@@ -857,72 +779,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>151</v>
       </c>
       <c r="C2" t="n">
-        <v>136</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.043</v>
+        <v>-0.127</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>143</v>
       </c>
       <c r="C3" t="n">
-        <v>143</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.114</v>
+        <v>-0.12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>114</v>
       </c>
       <c r="C4" t="n">
-        <v>108</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.369</v>
+        <v>0.395</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>144</v>
       </c>
       <c r="C5" t="n">
-        <v>142</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.179</v>
+        <v>-0.116</v>
       </c>
     </row>
   </sheetData>
@@ -941,72 +848,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>98</v>
       </c>
       <c r="C2" t="n">
-        <v>88</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.061</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>56</v>
       </c>
       <c r="C3" t="n">
-        <v>61</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.33</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>97</v>
       </c>
       <c r="C4" t="n">
-        <v>94</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.153</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>94</v>
       </c>
       <c r="C5" t="n">
-        <v>84</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.073</v>
+        <v>-0.123</v>
       </c>
     </row>
   </sheetData>
@@ -1025,71 +917,56 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>763</v>
       </c>
       <c r="C2" t="n">
-        <v>756</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.365</v>
+        <v>0.353</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>63</v>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.184</v>
+        <v>-0.171</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>79</v>
       </c>
       <c r="C4" t="n">
-        <v>76</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.207</v>
+        <v>-0.202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>54</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
-      </c>
-      <c r="D5" t="n">
         <v>-0.193</v>
       </c>
     </row>
@@ -1109,72 +986,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>68</v>
       </c>
       <c r="C2" t="n">
-        <v>65</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.196</v>
+        <v>-0.175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>740</v>
       </c>
       <c r="C3" t="n">
-        <v>724</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.402</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>84</v>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.24</v>
+        <v>-0.237</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>74</v>
       </c>
       <c r="C5" t="n">
-        <v>74</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.198</v>
+        <v>-0.18</v>
       </c>
     </row>
   </sheetData>
@@ -1193,72 +1055,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>83</v>
       </c>
       <c r="C2" t="n">
-        <v>78</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.2</v>
+        <v>-0.185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>705</v>
       </c>
       <c r="C3" t="n">
-        <v>692</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.415</v>
+        <v>0.391</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>74</v>
       </c>
       <c r="C4" t="n">
-        <v>73</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.219</v>
+        <v>-0.221</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>97</v>
       </c>
       <c r="C5" t="n">
-        <v>90</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.228</v>
+        <v>-0.204</v>
       </c>
     </row>
   </sheetData>
@@ -1277,72 +1124,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>107</v>
       </c>
       <c r="C2" t="n">
-        <v>108</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.234</v>
+        <v>-0.206</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>123</v>
       </c>
       <c r="C3" t="n">
-        <v>119</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.217</v>
+        <v>-0.204</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>97</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.125</v>
+        <v>-0.135</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="n">
+        <v>622</v>
       </c>
       <c r="C5" t="n">
-        <v>612</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.389</v>
+        <v>0.368</v>
       </c>
     </row>
   </sheetData>
@@ -1361,72 +1193,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>109</v>
       </c>
       <c r="C2" t="n">
-        <v>105</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.228</v>
+        <v>-0.212</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>133</v>
       </c>
       <c r="C3" t="n">
-        <v>130</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.212</v>
+        <v>-0.195</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>588</v>
       </c>
       <c r="C4" t="n">
-        <v>573</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.426</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>116</v>
       </c>
       <c r="C5" t="n">
-        <v>110</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.184</v>
+        <v>-0.185</v>
       </c>
     </row>
   </sheetData>
@@ -1445,72 +1262,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>126</v>
       </c>
       <c r="C2" t="n">
-        <v>116</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.165</v>
+        <v>-0.163</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>138</v>
       </c>
       <c r="C3" t="n">
-        <v>135</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.205</v>
+        <v>-0.187</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>541</v>
       </c>
       <c r="C4" t="n">
-        <v>528</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.42</v>
+        <v>0.392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>136</v>
       </c>
       <c r="C5" t="n">
-        <v>121</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.229</v>
+        <v>-0.206</v>
       </c>
     </row>
   </sheetData>
@@ -1529,72 +1331,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>146</v>
       </c>
       <c r="C2" t="n">
-        <v>142</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.167</v>
+        <v>-0.156</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>490</v>
       </c>
       <c r="C3" t="n">
-        <v>467</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.41</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>139</v>
       </c>
       <c r="C4" t="n">
-        <v>134</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.21</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>153</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.183</v>
+        <v>-0.174</v>
       </c>
     </row>
   </sheetData>
@@ -1613,72 +1400,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>145</v>
       </c>
       <c r="C2" t="n">
-        <v>143</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.181</v>
+        <v>-0.194</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>161</v>
       </c>
       <c r="C3" t="n">
-        <v>157</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.191</v>
+        <v>-0.137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>431</v>
       </c>
       <c r="C4" t="n">
-        <v>400</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.395</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>187</v>
       </c>
       <c r="C5" t="n">
-        <v>179</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.142</v>
+        <v>-0.139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>